<commit_message>
refactored code to specifiy upper bounds
</commit_message>
<xml_diff>
--- a/results/table_results_format.xlsx
+++ b/results/table_results_format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfairley/Projects/AdaptiveSurveillance/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1A5C69-4ADA-284A-AD84-8CA2816B2FB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83999AC3-9BC1-2549-BBA8-63AB63566AC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="26680" xr2:uid="{56335B14-10B7-A446-AC20-E8A18F2E0E77}"/>
   </bookViews>
@@ -34,17 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
-  <si>
-    <t>\Gamma = 1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
   <si>
     <t>False Alarm Probability</t>
   </si>
   <si>
-    <t>\Gamma = 50</t>
-  </si>
-  <si>
     <t>Algorithm</t>
   </si>
   <si>
@@ -60,18 +54,9 @@
     <t>Uniform Random</t>
   </si>
   <si>
-    <t>p_1^0</t>
-  </si>
-  <si>
-    <t>p_2^0</t>
-  </si>
-  <si>
     <t>0.00 [0.00, 0.00]</t>
   </si>
   <si>
-    <t>0.04 [0.02, 0.05]</t>
-  </si>
-  <si>
     <t>48 [48, 50]</t>
   </si>
   <si>
@@ -93,18 +78,12 @@
     <t>59 [58, 59]</t>
   </si>
   <si>
-    <t>0.00 [0.00, 0.01]</t>
-  </si>
-  <si>
     <t>84 [83, 85]</t>
   </si>
   <si>
     <t>71 [70, 72]</t>
   </si>
   <si>
-    <t>0.01 [0.00, 0.02]</t>
-  </si>
-  <si>
     <t>70 [69, 71]</t>
   </si>
   <si>
@@ -114,36 +93,24 @@
     <t>91 [89, 93]</t>
   </si>
   <si>
-    <t>NA [NA, NA]</t>
-  </si>
-  <si>
     <t>84 [83, 86]</t>
   </si>
   <si>
     <t>71 [69, 72]</t>
   </si>
   <si>
-    <t>0.07 [0.05, 0.08]</t>
-  </si>
-  <si>
     <t>38 [37, 39]</t>
   </si>
   <si>
     <t>30 [29, 30]</t>
   </si>
   <si>
-    <t>0.02 [0.01, 0.03]</t>
-  </si>
-  <si>
     <t>55 [54, 56]</t>
   </si>
   <si>
     <t>44 [43, 45]</t>
   </si>
   <si>
-    <t>0.03 [0.02, 0.04]</t>
-  </si>
-  <si>
     <t>45 [44, 45]</t>
   </si>
   <si>
@@ -153,10 +120,55 @@
     <t>56 [55, 57]</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Median Conditional Delay</t>
+  </si>
+  <si>
+    <t>0.04 [0.03, 0.04]</t>
+  </si>
+  <si>
+    <t>0.08 [0.07, 0.09]</t>
+  </si>
+  <si>
+    <t>0.05 [0.04, 0.06]</t>
+  </si>
+  <si>
+    <t>0.06 [0.06, 0.07]</t>
+  </si>
+  <si>
+    <t>0.06 [0.05, 0.07]</t>
+  </si>
+  <si>
+    <t>0.11 [0.10, 0.12]</t>
+  </si>
+  <si>
+    <t>0.18 [0.16, 0.19]</t>
+  </si>
+  <si>
+    <t>127 [121, 134]</t>
+  </si>
+  <si>
+    <t>0.07 [0.07, 0.08]</t>
+  </si>
+  <si>
+    <t>0.07 [0.06, 0.07]</t>
+  </si>
+  <si>
+    <t>0.02 [0.02, 0.03]</t>
+  </si>
+  <si>
+    <t>0.03 [0.03, 0.04]</t>
+  </si>
+  <si>
+    <t>$p_1^0$</t>
+  </si>
+  <si>
+    <t>$p_2^0$</t>
+  </si>
+  <si>
+    <t>$\Gamma_l = 1$</t>
+  </si>
+  <si>
+    <t>$\Gamma_l = 50$</t>
   </si>
 </sst>
 </file>
@@ -215,15 +227,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -543,7 +561,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -558,276 +576,276 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="5"/>
+      <c r="D1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="F5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="D8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="B3" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="D11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="4" t="s">
+      <c r="F13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="4" t="s">
+      <c r="D14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="B7" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="4" t="s">
+      <c r="G14" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
-        <v>0.02</v>
-      </c>
-      <c r="B11" s="3">
-        <v>0.01</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>